<commit_message>
After changing the computer
</commit_message>
<xml_diff>
--- a/_AAJ-PersonalMacroBook.xlsx
+++ b/_AAJ-PersonalMacroBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\404-Github\003-Excel High and Low\Excel_Guire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE2BC5FF-6D63-42CD-936E-1A2870C897C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3266EED-9497-4936-B7D1-DBEE3E80899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6FDE5474-AA63-4223-A0F5-80B999FD739B}"/>
   </bookViews>
@@ -36,11 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>This is a personal macrobook</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,16 +409,12 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>